<commit_message>
subdivide policy unit based on /24 prefixes
</commit_message>
<xml_diff>
--- a/eval/gatech.xlsx
+++ b/eval/gatech.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9560" yWindow="0" windowWidth="33600" windowHeight="19220" tabRatio="500" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="8600" yWindow="500" windowWidth="33600" windowHeight="19120" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="basic" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="119">
   <si>
     <t xml:space="preserve">GaTechrich-702 </t>
   </si>
@@ -309,6 +309,9 @@
     <t>room_str</t>
   </si>
   <si>
+    <t>os</t>
+  </si>
+  <si>
     <t>VLAN_routing</t>
   </si>
   <si>
@@ -376,6 +379,9 @@
   </si>
   <si>
     <t>#Attributes</t>
+  </si>
+  <si>
+    <t>Purdue_nonsubnet</t>
   </si>
 </sst>
 </file>
@@ -502,7 +508,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="340">
+  <cellStyleXfs count="358">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -843,6 +849,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -853,7 +877,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="21"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="25"/>
   </cellXfs>
-  <cellStyles count="340">
+  <cellStyles count="358">
     <cellStyle name="Bad" xfId="22" builtinId="27"/>
     <cellStyle name="Explanatory Text" xfId="25" builtinId="53"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1023,6 +1047,15 @@
     <cellStyle name="Followed Hyperlink" xfId="335" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="337" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="339" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="341" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="343" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="345" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="347" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="349" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="351" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="353" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="355" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="357" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="21" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1191,6 +1224,15 @@
     <cellStyle name="Hyperlink" xfId="334" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="336" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="338" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="340" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="342" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="344" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="346" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="348" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="350" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="352" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="354" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="356" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="24" builtinId="20"/>
     <cellStyle name="Neutral" xfId="23" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2223,7 +2265,7 @@
                   <c:v>90.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.0</c:v>
+                  <c:v>63.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2268,13 +2310,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>55.0</c:v>
+                  <c:v>54.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>90.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.0</c:v>
+                  <c:v>63.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2448,7 +2490,7 @@
                   <c:v>1201.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>584.0</c:v>
+                  <c:v>610.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2493,7 +2535,7 @@
                   <c:v>1287.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>615.0</c:v>
+                  <c:v>629.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2538,7 +2580,7 @@
                   <c:v>1287.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>753.0</c:v>
+                  <c:v>767.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2667,7 +2709,7 @@
                   <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.0</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2712,7 +2754,7 @@
                   <c:v>33.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.0</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2757,7 +2799,7 @@
                   <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.0</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2802,7 +2844,7 @@
                   <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.0</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5210,7 +5252,7 @@
                   <c:v>549.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>290.0</c:v>
+                  <c:v>800.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1334.0</c:v>
@@ -6772,8 +6814,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2055271000"/>
-        <c:axId val="-2090543912"/>
+        <c:axId val="-2050737112"/>
+        <c:axId val="-2055008728"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="-2055271000"/>
@@ -6808,6 +6850,37 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="-2055008728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2050737112"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="-2050737112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2055008728"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -10552,16 +10625,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10612,16 +10685,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1346200</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10642,16 +10715,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18349,20 +18422,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T80"/>
+  <dimension ref="A1:AS80"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:G14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:43">
       <c r="A1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:43">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -18379,7 +18452,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:43">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -18441,7 +18514,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:43">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -18505,7 +18578,7 @@
         <v>5064</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:43">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -18513,7 +18586,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:43">
       <c r="B6" t="s">
         <v>40</v>
       </c>
@@ -18551,7 +18624,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:43">
       <c r="B7">
         <f>B4</f>
         <v>4010</v>
@@ -18597,12 +18670,35 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:43">
       <c r="A8" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="W8" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="6"/>
+      <c r="AK8" s="6"/>
+      <c r="AL8" s="6"/>
+      <c r="AM8" s="6"/>
+      <c r="AN8" s="6"/>
+      <c r="AO8" s="6"/>
+      <c r="AP8" s="6"/>
+      <c r="AQ8" s="6"/>
+    </row>
+    <row r="9" spans="1:43">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -18618,8 +18714,39 @@
       <c r="O9" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:20">
+      <c r="W9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG9" s="6"/>
+      <c r="AH9" s="6"/>
+      <c r="AI9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ9" s="6"/>
+      <c r="AK9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL9" s="6"/>
+      <c r="AM9" s="6"/>
+      <c r="AN9" s="6"/>
+      <c r="AO9" s="6"/>
+      <c r="AP9" s="6"/>
+      <c r="AQ9" s="6"/>
+    </row>
+    <row r="10" spans="1:43">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -18680,8 +18807,69 @@
       <c r="T10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="W10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="X10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC10" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AN10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ10" s="6"/>
+    </row>
+    <row r="11" spans="1:43">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -18689,71 +18877,159 @@
         <v>1553</v>
       </c>
       <c r="C11">
-        <v>584</v>
+        <v>610</v>
       </c>
       <c r="D11">
-        <v>1195</v>
+        <v>1172</v>
       </c>
       <c r="E11">
-        <v>2306</v>
+        <v>2204</v>
       </c>
       <c r="F11">
-        <v>1263</v>
+        <v>1223</v>
       </c>
       <c r="G11">
-        <v>577</v>
+        <v>597</v>
       </c>
       <c r="H11">
-        <v>1142</v>
+        <v>1156</v>
       </c>
       <c r="I11">
-        <v>615</v>
+        <v>629</v>
       </c>
       <c r="J11">
-        <v>577</v>
+        <v>597</v>
       </c>
       <c r="K11">
-        <v>1550</v>
+        <v>1530</v>
       </c>
       <c r="L11">
-        <v>753</v>
+        <v>767</v>
       </c>
       <c r="M11">
         <f>MIN(H11,J11)</f>
-        <v>577</v>
+        <v>597</v>
       </c>
       <c r="N11">
         <f>MIN(I11, L11)</f>
-        <v>615</v>
+        <v>629</v>
       </c>
       <c r="O11">
-        <v>1520188</v>
+        <v>2109500</v>
       </c>
       <c r="P11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q11">
-        <v>512</v>
+        <v>523</v>
       </c>
       <c r="R11">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="S11">
         <v>0</v>
       </c>
       <c r="T11">
+        <v>589312</v>
+      </c>
+      <c r="W11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="X11" s="6">
+        <v>1553</v>
+      </c>
+      <c r="Y11" s="6">
+        <v>584</v>
+      </c>
+      <c r="Z11" s="6">
+        <v>1195</v>
+      </c>
+      <c r="AA11" s="6">
+        <v>2306</v>
+      </c>
+      <c r="AB11" s="6">
+        <v>1263</v>
+      </c>
+      <c r="AC11" s="6">
+        <v>577</v>
+      </c>
+      <c r="AD11" s="6">
+        <v>1142</v>
+      </c>
+      <c r="AE11" s="6">
+        <v>615</v>
+      </c>
+      <c r="AF11" s="6">
+        <v>577</v>
+      </c>
+      <c r="AG11" s="6">
+        <v>1550</v>
+      </c>
+      <c r="AH11" s="6">
+        <v>753</v>
+      </c>
+      <c r="AI11" s="6">
+        <f>MIN(AD11,AF11)</f>
+        <v>577</v>
+      </c>
+      <c r="AJ11" s="6">
+        <f>MIN(AE11, AH11)</f>
+        <v>615</v>
+      </c>
+      <c r="AK11" s="6">
+        <v>1520188</v>
+      </c>
+      <c r="AL11" s="6">
+        <v>21</v>
+      </c>
+      <c r="AM11" s="6">
+        <v>512</v>
+      </c>
+      <c r="AN11" s="6">
+        <v>72</v>
+      </c>
+      <c r="AO11" s="6">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="6">
         <v>229377</v>
       </c>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="AQ11" s="6"/>
+    </row>
+    <row r="12" spans="1:43">
       <c r="A12" t="s">
         <v>82</v>
       </c>
       <c r="J12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="W12" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="6"/>
+      <c r="AE12" s="6"/>
+      <c r="AF12" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG12" s="6"/>
+      <c r="AH12" s="6"/>
+      <c r="AI12" s="6"/>
+      <c r="AJ12" s="6"/>
+      <c r="AK12" s="6"/>
+      <c r="AL12" s="6"/>
+      <c r="AM12" s="6"/>
+      <c r="AN12" s="6"/>
+      <c r="AO12" s="6"/>
+      <c r="AP12" s="6"/>
+      <c r="AQ12" s="6"/>
+    </row>
+    <row r="13" spans="1:43">
       <c r="B13" t="s">
         <v>40</v>
       </c>
@@ -18790,54 +19066,152 @@
       <c r="P13" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="W13" s="6"/>
+      <c r="X13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD13" s="6"/>
+      <c r="AE13" s="6"/>
+      <c r="AF13" s="6"/>
+      <c r="AG13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM13" s="6"/>
+      <c r="AN13" s="6"/>
+      <c r="AO13" s="6"/>
+      <c r="AP13" s="6"/>
+      <c r="AQ13" s="6"/>
+    </row>
+    <row r="14" spans="1:43">
       <c r="B14">
         <f>B11</f>
         <v>1553</v>
       </c>
       <c r="C14">
         <f>C11</f>
-        <v>584</v>
+        <v>610</v>
       </c>
       <c r="D14">
         <f>F11</f>
-        <v>1263</v>
+        <v>1223</v>
       </c>
       <c r="E14">
         <f>N11</f>
-        <v>615</v>
+        <v>629</v>
       </c>
       <c r="F14">
         <f>E11</f>
-        <v>2306</v>
+        <v>2204</v>
       </c>
       <c r="G14">
         <f>L11</f>
-        <v>753</v>
+        <v>767</v>
       </c>
       <c r="K14">
         <f>CEILING(LOG(O11,2),1)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L14">
         <f>CEILING(LOG(Q11,2),1) + CEILING(LOG(R11, 2), 1) + CEILING(LOG(T11,2),1)</f>
+        <v>37</v>
+      </c>
+      <c r="M14">
+        <v>22</v>
+      </c>
+      <c r="N14">
+        <v>23</v>
+      </c>
+      <c r="O14">
+        <v>22</v>
+      </c>
+      <c r="P14">
+        <v>23</v>
+      </c>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6">
+        <f>X11</f>
+        <v>1553</v>
+      </c>
+      <c r="Y14" s="6">
+        <f>Y11</f>
+        <v>584</v>
+      </c>
+      <c r="Z14" s="6">
+        <f>AB11</f>
+        <v>1263</v>
+      </c>
+      <c r="AA14" s="6">
+        <f>AJ11</f>
+        <v>615</v>
+      </c>
+      <c r="AB14" s="6">
+        <f>AA11</f>
+        <v>2306</v>
+      </c>
+      <c r="AC14" s="6">
+        <f>AH11</f>
+        <v>753</v>
+      </c>
+      <c r="AD14" s="6"/>
+      <c r="AE14" s="6"/>
+      <c r="AF14" s="6"/>
+      <c r="AG14" s="6">
+        <f>CEILING(LOG(AK11,2),1)</f>
+        <v>21</v>
+      </c>
+      <c r="AH14" s="6">
+        <f>CEILING(LOG(AM11,2),1) + CEILING(LOG(AN11, 2), 1) + CEILING(LOG(AP11,2),1)</f>
         <v>34</v>
       </c>
-      <c r="M14">
+      <c r="AI14" s="6">
         <v>21</v>
       </c>
-      <c r="N14">
+      <c r="AJ14" s="6">
         <v>22</v>
       </c>
-      <c r="O14">
+      <c r="AK14" s="6">
         <v>21</v>
       </c>
-      <c r="P14">
+      <c r="AL14" s="6">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="AM14" s="6"/>
+      <c r="AN14" s="6"/>
+      <c r="AO14" s="6"/>
+      <c r="AP14" s="6"/>
+      <c r="AQ14" s="6"/>
+    </row>
+    <row r="17" spans="1:45">
       <c r="A17" s="1" t="s">
         <v>78</v>
       </c>
@@ -18869,7 +19243,7 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:45">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -18931,7 +19305,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:45">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -18994,8 +19368,12 @@
       <c r="T19">
         <v>5064</v>
       </c>
-    </row>
-    <row r="20" spans="1:20">
+      <c r="V19">
+        <f>1-N19/B19</f>
+        <v>0.42903800475059384</v>
+      </c>
+    </row>
+    <row r="20" spans="1:45">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -19058,8 +19436,12 @@
       <c r="T20">
         <v>5064</v>
       </c>
-    </row>
-    <row r="21" spans="1:20">
+      <c r="V20">
+        <f t="shared" ref="V20:V35" si="2">1-N20/B20</f>
+        <v>0.45574886535552195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:45">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -19122,8 +19504,12 @@
       <c r="T21">
         <v>5064</v>
       </c>
-    </row>
-    <row r="22" spans="1:20">
+      <c r="V21">
+        <f t="shared" si="2"/>
+        <v>0.87012578616352199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:45">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -19186,8 +19572,12 @@
       <c r="T22">
         <v>5064</v>
       </c>
-    </row>
-    <row r="23" spans="1:20">
+      <c r="V22">
+        <f t="shared" si="2"/>
+        <v>0.55583437892095355</v>
+      </c>
+    </row>
+    <row r="23" spans="1:45">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -19250,8 +19640,12 @@
       <c r="T23">
         <v>5064</v>
       </c>
-    </row>
-    <row r="24" spans="1:20">
+      <c r="V23">
+        <f t="shared" si="2"/>
+        <v>0.39107142857142863</v>
+      </c>
+    </row>
+    <row r="24" spans="1:45">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -19314,8 +19708,12 @@
       <c r="T24">
         <v>5064</v>
       </c>
-    </row>
-    <row r="25" spans="1:20">
+      <c r="V24">
+        <f t="shared" si="2"/>
+        <v>0.95990099009900987</v>
+      </c>
+    </row>
+    <row r="25" spans="1:45">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -19378,8 +19776,12 @@
       <c r="T25">
         <v>5064</v>
       </c>
-    </row>
-    <row r="26" spans="1:20">
+      <c r="V25">
+        <f t="shared" si="2"/>
+        <v>0.54801967382863059</v>
+      </c>
+    </row>
+    <row r="26" spans="1:45">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -19442,8 +19844,12 @@
       <c r="T26">
         <v>5064</v>
       </c>
-    </row>
-    <row r="27" spans="1:20">
+      <c r="V26">
+        <f t="shared" si="2"/>
+        <v>0.90768605124034163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:45">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -19506,8 +19912,12 @@
       <c r="T27">
         <v>5064</v>
       </c>
-    </row>
-    <row r="28" spans="1:20">
+      <c r="V27">
+        <f t="shared" si="2"/>
+        <v>0.94069806845137238</v>
+      </c>
+    </row>
+    <row r="28" spans="1:45">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -19570,8 +19980,12 @@
       <c r="T28">
         <v>5064</v>
       </c>
-    </row>
-    <row r="29" spans="1:20">
+      <c r="V28">
+        <f t="shared" si="2"/>
+        <v>0.53703703703703698</v>
+      </c>
+    </row>
+    <row r="29" spans="1:45">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -19634,8 +20048,12 @@
       <c r="T29">
         <v>5064</v>
       </c>
-    </row>
-    <row r="30" spans="1:20">
+      <c r="V29">
+        <f t="shared" si="2"/>
+        <v>0.50075015444356197</v>
+      </c>
+    </row>
+    <row r="30" spans="1:45">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -19698,8 +20116,12 @@
       <c r="T30">
         <v>5064</v>
       </c>
-    </row>
-    <row r="31" spans="1:20">
+      <c r="V30">
+        <f t="shared" si="2"/>
+        <v>0.56474559922835788</v>
+      </c>
+    </row>
+    <row r="31" spans="1:45">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -19762,8 +20184,15 @@
       <c r="T31">
         <v>5064</v>
       </c>
-    </row>
-    <row r="32" spans="1:20">
+      <c r="V31">
+        <f t="shared" si="2"/>
+        <v>0.78193525931082486</v>
+      </c>
+      <c r="X31" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:45">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
@@ -19824,8 +20253,77 @@
       <c r="T32" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="1:20">
+      <c r="V32" t="e">
+        <f>1-N32/B32</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X32" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y32" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z32" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA32" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB32" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC32" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD32" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE32" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF32" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG32" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH32" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI32" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ32" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK32" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL32" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM32" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AN32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP32" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AQ32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR32" s="6"/>
+      <c r="AS32" s="6" t="e">
+        <f>1-AK32/Y32</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:45">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -19836,60 +20334,131 @@
         <v>54</v>
       </c>
       <c r="D33">
-        <v>181</v>
+        <v>304</v>
       </c>
       <c r="E33">
-        <v>378</v>
+        <v>326</v>
       </c>
       <c r="F33">
-        <v>187</v>
+        <v>304</v>
       </c>
       <c r="G33">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H33">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I33">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="J33">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K33">
-        <v>213</v>
+        <v>106</v>
       </c>
       <c r="L33">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M33">
         <f>MIN(H33,K33)</f>
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="N33">
         <f>MIN(I33,L33)</f>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O33">
-        <v>303967026</v>
+        <v>2109500</v>
       </c>
       <c r="P33">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="Q33">
-        <v>512</v>
+        <v>523</v>
       </c>
       <c r="R33">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="S33">
         <v>0</v>
       </c>
       <c r="T33">
+        <v>589312</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="2"/>
+        <v>0.9293193717277487</v>
+      </c>
+      <c r="X33" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y33" s="6">
+        <v>764</v>
+      </c>
+      <c r="Z33" s="6">
+        <v>54</v>
+      </c>
+      <c r="AA33" s="6">
+        <v>181</v>
+      </c>
+      <c r="AB33" s="6">
+        <v>378</v>
+      </c>
+      <c r="AC33" s="6">
+        <v>187</v>
+      </c>
+      <c r="AD33" s="6">
+        <v>55</v>
+      </c>
+      <c r="AE33" s="6">
+        <v>89</v>
+      </c>
+      <c r="AF33" s="6">
+        <v>64</v>
+      </c>
+      <c r="AG33" s="6">
+        <v>55</v>
+      </c>
+      <c r="AH33" s="6">
+        <v>213</v>
+      </c>
+      <c r="AI33" s="6">
+        <v>55</v>
+      </c>
+      <c r="AJ33" s="6">
+        <f>MIN(AE33,AH33)</f>
+        <v>89</v>
+      </c>
+      <c r="AK33" s="6">
+        <f>MIN(AF33,AI33)</f>
+        <v>55</v>
+      </c>
+      <c r="AL33" s="6">
+        <v>303967026</v>
+      </c>
+      <c r="AM33" s="6">
+        <v>29</v>
+      </c>
+      <c r="AN33" s="6">
+        <v>512</v>
+      </c>
+      <c r="AO33" s="6">
+        <v>72</v>
+      </c>
+      <c r="AP33" s="6">
+        <v>0</v>
+      </c>
+      <c r="AQ33" s="6">
         <v>234881014</v>
       </c>
-    </row>
-    <row r="34" spans="1:20">
+      <c r="AR33" s="6"/>
+      <c r="AS33" s="6">
+        <f t="shared" ref="AS33:AS35" si="3">1-AK33/Y33</f>
+        <v>0.92801047120418845</v>
+      </c>
+    </row>
+    <row r="34" spans="1:45">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -19900,60 +20469,131 @@
         <v>90</v>
       </c>
       <c r="D34">
-        <v>2281</v>
+        <v>720</v>
       </c>
       <c r="E34">
-        <v>6992</v>
+        <v>1448</v>
       </c>
       <c r="F34">
-        <v>2492</v>
+        <v>741</v>
       </c>
       <c r="G34">
         <v>90</v>
       </c>
       <c r="H34">
-        <v>731</v>
+        <v>660</v>
       </c>
       <c r="I34">
-        <v>362</v>
+        <v>90</v>
       </c>
       <c r="J34">
         <v>90</v>
       </c>
       <c r="K34">
-        <v>5879</v>
+        <v>1243</v>
       </c>
       <c r="L34">
+        <v>200</v>
+      </c>
+      <c r="M34">
+        <f t="shared" ref="M34:M35" si="4">MIN(H34,K34)</f>
+        <v>660</v>
+      </c>
+      <c r="N34">
+        <f t="shared" ref="N34:N35" si="5">MIN(I34,L34)</f>
         <v>90</v>
       </c>
-      <c r="M34">
-        <f t="shared" ref="M34:M35" si="2">MIN(H34,K34)</f>
-        <v>731</v>
-      </c>
-      <c r="N34">
-        <f t="shared" ref="N34:N35" si="3">MIN(I34,L34)</f>
-        <v>90</v>
-      </c>
       <c r="O34">
-        <v>303967026</v>
+        <v>2109500</v>
       </c>
       <c r="P34">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="Q34">
-        <v>512</v>
+        <v>523</v>
       </c>
       <c r="R34">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="S34">
         <v>0</v>
       </c>
       <c r="T34">
+        <v>589312</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="2"/>
+        <v>0.65116279069767447</v>
+      </c>
+      <c r="X34" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y34" s="6">
+        <v>258</v>
+      </c>
+      <c r="Z34" s="6">
+        <v>90</v>
+      </c>
+      <c r="AA34" s="6">
+        <v>2281</v>
+      </c>
+      <c r="AB34" s="6">
+        <v>6992</v>
+      </c>
+      <c r="AC34" s="6">
+        <v>2492</v>
+      </c>
+      <c r="AD34" s="6">
+        <v>90</v>
+      </c>
+      <c r="AE34" s="6">
+        <v>731</v>
+      </c>
+      <c r="AF34" s="6">
+        <v>362</v>
+      </c>
+      <c r="AG34" s="6">
+        <v>90</v>
+      </c>
+      <c r="AH34" s="6">
+        <v>5879</v>
+      </c>
+      <c r="AI34" s="6">
+        <v>90</v>
+      </c>
+      <c r="AJ34" s="6">
+        <f t="shared" ref="AJ34:AJ35" si="6">MIN(AE34,AH34)</f>
+        <v>731</v>
+      </c>
+      <c r="AK34" s="6">
+        <f t="shared" ref="AK34:AK35" si="7">MIN(AF34,AI34)</f>
+        <v>90</v>
+      </c>
+      <c r="AL34" s="6">
+        <v>303967026</v>
+      </c>
+      <c r="AM34" s="6">
+        <v>29</v>
+      </c>
+      <c r="AN34" s="6">
+        <v>512</v>
+      </c>
+      <c r="AO34" s="6">
+        <v>72</v>
+      </c>
+      <c r="AP34" s="6">
+        <v>0</v>
+      </c>
+      <c r="AQ34" s="6">
         <v>234881014</v>
       </c>
-    </row>
-    <row r="35" spans="1:20">
+      <c r="AR34" s="6"/>
+      <c r="AS34" s="6">
+        <f t="shared" si="3"/>
+        <v>0.65116279069767447</v>
+      </c>
+    </row>
+    <row r="35" spans="1:45">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -19961,63 +20601,134 @@
         <v>131</v>
       </c>
       <c r="C35">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D35">
-        <v>1630</v>
+        <v>406</v>
       </c>
       <c r="E35">
-        <v>5008</v>
+        <v>738</v>
       </c>
       <c r="F35">
-        <v>1798</v>
+        <v>406</v>
       </c>
       <c r="G35">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="H35">
-        <v>444</v>
+        <v>403</v>
       </c>
       <c r="I35">
-        <v>219</v>
+        <v>63</v>
       </c>
       <c r="J35">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="K35">
-        <v>3540</v>
+        <v>741</v>
       </c>
       <c r="L35">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="M35">
-        <f t="shared" si="2"/>
-        <v>444</v>
+        <f t="shared" si="4"/>
+        <v>403</v>
       </c>
       <c r="N35">
-        <f t="shared" si="3"/>
-        <v>55</v>
+        <f t="shared" si="5"/>
+        <v>63</v>
       </c>
       <c r="O35">
-        <v>303967026</v>
+        <v>2109500</v>
       </c>
       <c r="P35">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="Q35">
-        <v>512</v>
+        <v>523</v>
       </c>
       <c r="R35">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="S35">
         <v>0</v>
       </c>
       <c r="T35">
+        <v>589312</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="2"/>
+        <v>0.51908396946564883</v>
+      </c>
+      <c r="X35" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y35" s="6">
+        <v>131</v>
+      </c>
+      <c r="Z35" s="6">
+        <v>55</v>
+      </c>
+      <c r="AA35" s="6">
+        <v>1630</v>
+      </c>
+      <c r="AB35" s="6">
+        <v>5008</v>
+      </c>
+      <c r="AC35" s="6">
+        <v>1798</v>
+      </c>
+      <c r="AD35" s="6">
+        <v>55</v>
+      </c>
+      <c r="AE35" s="6">
+        <v>444</v>
+      </c>
+      <c r="AF35" s="6">
+        <v>219</v>
+      </c>
+      <c r="AG35" s="6">
+        <v>55</v>
+      </c>
+      <c r="AH35" s="6">
+        <v>3540</v>
+      </c>
+      <c r="AI35" s="6">
+        <v>55</v>
+      </c>
+      <c r="AJ35" s="6">
+        <f t="shared" si="6"/>
+        <v>444</v>
+      </c>
+      <c r="AK35" s="6">
+        <f t="shared" si="7"/>
+        <v>55</v>
+      </c>
+      <c r="AL35" s="6">
+        <v>303967026</v>
+      </c>
+      <c r="AM35" s="6">
+        <v>29</v>
+      </c>
+      <c r="AN35" s="6">
+        <v>512</v>
+      </c>
+      <c r="AO35" s="6">
+        <v>72</v>
+      </c>
+      <c r="AP35" s="6">
+        <v>0</v>
+      </c>
+      <c r="AQ35" s="6">
         <v>234881014</v>
       </c>
-    </row>
-    <row r="39" spans="1:20">
+      <c r="AR35" s="6"/>
+      <c r="AS35" s="6">
+        <f t="shared" si="3"/>
+        <v>0.58015267175572527</v>
+      </c>
+    </row>
+    <row r="39" spans="1:45">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -20040,7 +20751,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:45">
       <c r="A40" t="str">
         <f>A19</f>
         <v xml:space="preserve">GaTech134 </v>
@@ -20070,7 +20781,7 @@
         <v>52221</v>
       </c>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:45">
       <c r="A41" t="str">
         <f>A20</f>
         <v xml:space="preserve">GaTech160 </v>
@@ -20100,7 +20811,7 @@
         <v>58624</v>
       </c>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:45">
       <c r="A42" t="str">
         <f>A21</f>
         <v xml:space="preserve">GaTech161 </v>
@@ -20130,7 +20841,7 @@
         <v>8462</v>
       </c>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:45">
       <c r="A43" t="str">
         <f>A22</f>
         <v xml:space="preserve">GaTech1901 </v>
@@ -20160,7 +20871,7 @@
         <v>150602</v>
       </c>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:45">
       <c r="A44" t="str">
         <f>A23</f>
         <v xml:space="preserve">GaTech209 </v>
@@ -20190,7 +20901,7 @@
         <v>71560</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:45">
       <c r="A45" t="str">
         <f>A24</f>
         <v xml:space="preserve">GaTech411 </v>
@@ -20220,7 +20931,7 @@
         <v>7762</v>
       </c>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:45">
       <c r="A46" t="str">
         <f>A25</f>
         <v xml:space="preserve">GaTech47 </v>
@@ -20250,7 +20961,7 @@
         <v>15601</v>
       </c>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:45">
       <c r="A47" t="str">
         <f>A26</f>
         <v xml:space="preserve">GaTech499 </v>
@@ -20280,7 +20991,7 @@
         <v>1545</v>
       </c>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:45">
       <c r="A48" t="str">
         <f>A27</f>
         <v xml:space="preserve">GaTech691 </v>
@@ -20432,15 +21143,15 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="str">
-        <f t="shared" ref="A53:C53" si="4">A32</f>
+        <f t="shared" ref="A53:C53" si="8">A32</f>
         <v>name</v>
       </c>
       <c r="B53" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>Original</v>
       </c>
       <c r="C53" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>BitSegmentation</v>
       </c>
       <c r="D53" t="str">
@@ -20462,45 +21173,45 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="str">
-        <f t="shared" ref="A54:C54" si="5">A33</f>
+        <f t="shared" ref="A54:C54" si="9">A33</f>
         <v xml:space="preserve"> UN9airtmGppdzE </v>
       </c>
       <c r="B54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>764</v>
       </c>
       <c r="C54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>54</v>
       </c>
       <c r="D54">
         <f>N33</f>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E54">
         <f>L33</f>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F54">
         <f>F33</f>
-        <v>187</v>
+        <v>304</v>
       </c>
       <c r="G54">
         <f>E33</f>
-        <v>378</v>
+        <v>326</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="str">
-        <f t="shared" ref="A55:C55" si="6">A34</f>
+        <f t="shared" ref="A55:C55" si="10">A34</f>
         <v xml:space="preserve"> 621TrDEEO6ku2N </v>
       </c>
       <c r="B55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>258</v>
       </c>
       <c r="C55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>90</v>
       </c>
       <c r="D55">
@@ -20509,45 +21220,45 @@
       </c>
       <c r="E55">
         <f>L34</f>
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="F55">
         <f>F34</f>
-        <v>2492</v>
+        <v>741</v>
       </c>
       <c r="G55">
         <f>E34</f>
-        <v>6992</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="str">
-        <f t="shared" ref="A56:C56" si="7">A35</f>
+        <f t="shared" ref="A56:C56" si="11">A35</f>
         <v xml:space="preserve"> ryK+HUNAcKibEDb </v>
       </c>
       <c r="B56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>131</v>
       </c>
       <c r="C56">
-        <f t="shared" si="7"/>
-        <v>55</v>
+        <f t="shared" si="11"/>
+        <v>63</v>
       </c>
       <c r="D56">
         <f>N35</f>
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E56">
         <f>L35</f>
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="F56">
         <f>F35</f>
-        <v>1798</v>
+        <v>406</v>
       </c>
       <c r="G56">
         <f>E35</f>
-        <v>5008</v>
+        <v>738</v>
       </c>
     </row>
     <row r="75" spans="1:16">
@@ -20587,7 +21298,7 @@
         <v>13</v>
       </c>
       <c r="G76">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
@@ -20607,7 +21318,7 @@
         <v>1201</v>
       </c>
       <c r="C77">
-        <v>584</v>
+        <v>610</v>
       </c>
       <c r="E77" t="s">
         <v>41</v>
@@ -20616,7 +21327,7 @@
         <v>33</v>
       </c>
       <c r="G77">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
@@ -20636,7 +21347,7 @@
         <v>1287</v>
       </c>
       <c r="C78">
-        <v>615</v>
+        <v>629</v>
       </c>
       <c r="E78" t="s">
         <v>47</v>
@@ -20645,7 +21356,7 @@
         <v>14</v>
       </c>
       <c r="G78">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="79" spans="1:16">
@@ -20656,7 +21367,7 @@
         <v>1287</v>
       </c>
       <c r="C79" s="1">
-        <v>753</v>
+        <v>767</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1" t="s">
@@ -20666,7 +21377,7 @@
         <v>14</v>
       </c>
       <c r="G79" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="80" spans="1:16">
@@ -20693,7 +21404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
@@ -42232,8 +42943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" activeCellId="1" sqref="A26:C33 F26:F33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -42245,7 +42956,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -42305,9 +43016,11 @@
         <v>46</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q4" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
     </row>
@@ -42357,6 +43070,9 @@
       <c r="O5">
         <v>8</v>
       </c>
+      <c r="Q5">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
@@ -42404,6 +43120,9 @@
       <c r="O6">
         <v>1499</v>
       </c>
+      <c r="Q6">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
@@ -42451,6 +43170,9 @@
       <c r="O7">
         <v>1499</v>
       </c>
+      <c r="Q7">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" t="s">
@@ -42498,6 +43220,9 @@
       <c r="O8">
         <v>1499</v>
       </c>
+      <c r="Q8">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
@@ -42540,10 +43265,13 @@
         <v>290</v>
       </c>
       <c r="N9">
-        <v>290</v>
+        <v>800</v>
       </c>
       <c r="O9">
         <v>1499</v>
+      </c>
+      <c r="Q9">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -42592,20 +43320,30 @@
       <c r="O10">
         <v>1499</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" s="6" customFormat="1"/>
+      <c r="Q10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" s="6" customFormat="1">
+      <c r="A11" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>5</v>
+      </c>
+    </row>
     <row r="12" spans="1:19" s="6" customFormat="1"/>
     <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B16" t="s">
         <v>47</v>
@@ -42620,7 +43358,7 @@
         <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -42766,10 +43504,10 @@
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" t="s">
         <v>107</v>
-      </c>
-      <c r="B25" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -42786,15 +43524,15 @@
         <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B27">
         <v>136</v>
@@ -42817,7 +43555,7 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B28">
         <v>120</v>
@@ -42844,7 +43582,7 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B29">
         <v>96</v>
@@ -42867,7 +43605,7 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B30">
         <v>85</v>
@@ -42897,7 +43635,7 @@
     </row>
     <row r="31" spans="1:15">
       <c r="A31" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B31">
         <v>59</v>
@@ -42921,7 +43659,7 @@
     </row>
     <row r="32" spans="1:15">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B32">
         <v>49</v>
@@ -42944,7 +43682,7 @@
     </row>
     <row r="33" spans="1:14">
       <c r="A33" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B33">
         <v>34</v>
@@ -42973,12 +43711,12 @@
     </row>
     <row r="44" spans="1:14">
       <c r="A44" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:14">
       <c r="B45" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -42996,7 +43734,7 @@
         <v>4</v>
       </c>
       <c r="H45" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J45">
         <v>0</v>
@@ -43016,34 +43754,34 @@
     </row>
     <row r="46" spans="1:14">
       <c r="C46" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D46" t="s">
+        <v>97</v>
+      </c>
+      <c r="E46" t="s">
+        <v>98</v>
+      </c>
+      <c r="F46" t="s">
+        <v>99</v>
+      </c>
+      <c r="G46" t="s">
+        <v>102</v>
+      </c>
+      <c r="J46" t="s">
         <v>96</v>
       </c>
-      <c r="E46" t="s">
+      <c r="K46" t="s">
         <v>97</v>
       </c>
-      <c r="F46" t="s">
+      <c r="L46" t="s">
         <v>98</v>
       </c>
-      <c r="G46" t="s">
-        <v>101</v>
-      </c>
-      <c r="J46" t="s">
-        <v>95</v>
-      </c>
-      <c r="K46" t="s">
-        <v>96</v>
-      </c>
-      <c r="L46" t="s">
-        <v>97</v>
-      </c>
       <c r="M46" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N46" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -43051,7 +43789,7 @@
         <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D47">
         <v>21260</v>
@@ -43069,7 +43807,7 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K47">
         <v>137886</v>
@@ -43089,7 +43827,7 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E48">
         <v>45583</v>
@@ -43104,7 +43842,7 @@
         <v>1</v>
       </c>
       <c r="I48" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L48">
         <v>221837</v>
@@ -43121,7 +43859,7 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F49">
         <v>3497</v>
@@ -43133,7 +43871,7 @@
         <v>2</v>
       </c>
       <c r="I49" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M49">
         <v>31691</v>
@@ -43147,7 +43885,7 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G50">
         <v>2688</v>
@@ -43156,7 +43894,7 @@
         <v>3</v>
       </c>
       <c r="I50" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N50">
         <v>12596</v>
@@ -43167,18 +43905,18 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H51">
         <v>4</v>
       </c>
       <c r="I51" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:14">
       <c r="A53" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -43198,19 +43936,19 @@
     </row>
     <row r="54" spans="1:14">
       <c r="C54" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D54" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E54" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F54" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G54" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:14">
@@ -43218,7 +43956,7 @@
         <v>0</v>
       </c>
       <c r="B55" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D55">
         <f>D47/K47</f>
@@ -43242,7 +43980,7 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E56">
         <f t="shared" si="1"/>
@@ -43262,7 +44000,7 @@
         <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F57">
         <f t="shared" si="3"/>
@@ -43278,7 +44016,7 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G58">
         <f t="shared" si="4"/>
@@ -43290,7 +44028,7 @@
         <v>4</v>
       </c>
       <c r="B59" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>